<commit_message>
Added "updated" date to assessment
This will help keep track of versioning, and knowing how old a saved copy of the self assessment is. :)
</commit_message>
<xml_diff>
--- a/Assessments/Exam-Msft-AZ-103-Self-Assessment-Build5Nines.xlsx
+++ b/Assessments/Exam-Msft-AZ-103-Self-Assessment-Build5Nines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_2060\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="474" documentId="11_D9DEADA52AFC04C703D00068A70CDD6EE27F7719" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BB15BE58-AEF7-414E-AD60-66552FA35636}"/>
+  <xr:revisionPtr revIDLastSave="477" documentId="11_D9DEADA52AFC04C703D00068A70CDD6EE27F7719" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{82363136-496F-4867-B9EB-F9720FC7B37E}"/>
   <bookViews>
     <workbookView xWindow="165" yWindow="23505" windowWidth="29160" windowHeight="18300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="160">
   <si>
     <t>Microsoft Certification Self-Assessment Tool</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>Keep in mind that all exam Objective Domain info/text is copyright by Microsoft.</t>
+  </si>
+  <si>
+    <t>Self Assessment last updated November 11, 2019</t>
   </si>
   <si>
     <t>Objective Domain</t>
@@ -519,7 +522,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -640,6 +643,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -690,7 +701,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -710,6 +721,7 @@
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2646,10 +2658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAC8EB29-E03A-442E-8AA1-F3DC81B6E73C}">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2831,6 +2843,11 @@
     <row r="34" spans="1:1">
       <c r="A34" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="19" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -2911,16 +2928,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="14" customFormat="1" ht="18.75">
       <c r="A1" s="14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="6" customFormat="1" ht="21">
@@ -2934,7 +2951,7 @@
     </row>
     <row r="3" spans="1:4" s="7" customFormat="1" ht="18.75">
       <c r="B3" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D3" s="8">
         <f>(IF(D4="Know Well", 1, IF(D4="Know a Little", 0.5, 0))+IF(D5="Know Well", 1, IF(D5="Know a Little", 0.5, 0))+IF(D6="Know Well", 1, IF(D6="Know a Little", 0.5, 0)))/3</f>
@@ -2943,31 +2960,31 @@
     </row>
     <row r="4" spans="1:4" ht="15.75">
       <c r="C4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75">
       <c r="C5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75">
       <c r="C6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="7" customFormat="1" ht="18.75">
       <c r="B7" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D7" s="8">
         <f>(IF(D8="Know Well", 1, IF(D8="Know a Little", 0.5, 0))+IF(D9="Know Well", 1, IF(D9="Know a Little", 0.5, 0))+IF(D10="Know Well", 1, IF(D10="Know a Little", 0.5, 0))+IF(D11="Know Well", 1, IF(D11="Know a Little", 0.5, 0))+IF(D12="Know Well", 1, IF(D12="Know a Little", 0.5, 0))+IF(D13="Know Well", 1, IF(D13="Know a Little", 0.5, 0))+IF(D14="Know Well", 1, IF(D14="Know a Little", 0.5, 0))+IF(D15="Know Well", 1, IF(D15="Know a Little", 0.5, 0))+IF(D16="Know Well", 1, IF(D16="Know a Little", 0.5, 0))+IF(D17="Know Well", 1, IF(D17="Know a Little", 0.5, 0))+IF(D18="Know Well", 1, IF(D18="Know a Little", 0.5, 0)))/11</f>
@@ -2976,95 +2993,95 @@
     </row>
     <row r="8" spans="1:4" ht="15.75">
       <c r="C8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75">
       <c r="C9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75">
       <c r="C10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75">
       <c r="C11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75">
       <c r="C12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75">
       <c r="C13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75">
       <c r="C14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75">
       <c r="C15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75">
       <c r="C16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75">
       <c r="C17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75">
       <c r="C18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="7" customFormat="1" ht="18.75">
       <c r="B19" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D19" s="8">
         <f>(IF(D20="Know Well", 1, IF(D20="Know a Little", 0.5, 0))+IF(D21="Know Well", 1, IF(D21="Know a Little", 0.5, 0))+IF(D22="Know Well", 1, IF(D22="Know a Little", 0.5, 0))+IF(D23="Know Well", 1, IF(D23="Know a Little", 0.5, 0))+IF(D24="Know Well", 1, IF(D24="Know a Little", 0.5, 0))+IF(D25="Know Well", 1, IF(D25="Know a Little", 0.5, 0))+IF(D26="Know Well", 1, IF(D26="Know a Little", 0.5, 0)))/7</f>
@@ -3073,63 +3090,63 @@
     </row>
     <row r="20" spans="1:4" ht="15.75">
       <c r="C20" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D20" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75">
       <c r="C21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D21" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75">
       <c r="C22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D22" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75">
       <c r="C23" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D23" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75">
       <c r="C24" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D24" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75">
       <c r="C25" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D25" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75">
       <c r="C26" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D26" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="7" customFormat="1" ht="18.75">
       <c r="B27" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D27" s="8">
         <f>(IF(D28="Know Well", 1, IF(D28="Know a Little", 0.5, 0))+IF(D29="Know Well", 1, IF(D29="Know a Little", 0.5, 0))+IF(D30="Know Well", 1, IF(D30="Know a Little", 0.5, 0)))/3</f>
@@ -3138,26 +3155,26 @@
     </row>
     <row r="28" spans="1:4" ht="15.75">
       <c r="C28" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D28" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75">
       <c r="C29" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D29" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75">
       <c r="C30" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D30" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="6" customFormat="1" ht="21">
@@ -3171,7 +3188,7 @@
     </row>
     <row r="32" spans="1:4" s="7" customFormat="1" ht="18.75">
       <c r="B32" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D32" s="8">
         <f>(IF(D33="Know Well", 1, IF(D33="Know a Little", 0.5, 0))+IF(D34="Know Well", 1, IF(D34="Know a Little", 0.5, 0))+IF(D35="Know Well", 1, IF(D35="Know a Little", 0.5, 0))+IF(D36="Know Well", 1, IF(D36="Know a Little", 0.5, 0))+IF(D37="Know Well", 1, IF(D37="Know a Little", 0.5, 0))+IF(D38="Know Well", 1, IF(D38="Know a Little", 0.5, 0))+IF(D39="Know Well", 1, IF(D39="Know a Little", 0.5, 0))+IF(D40="Know Well", 1, IF(D40="Know a Little", 0.5, 0)))/8</f>
@@ -3180,71 +3197,71 @@
     </row>
     <row r="33" spans="2:4" ht="15.75">
       <c r="C33" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D33" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="15.75">
       <c r="C34" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D34" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="15.75">
       <c r="C35" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D35" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="15.75">
       <c r="C36" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D36" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="15.75">
       <c r="C37" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D37" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="15.75">
       <c r="C38" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D38" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="15.75">
       <c r="C39" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D39" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="15.75">
       <c r="C40" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D40" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="2:4" s="7" customFormat="1" ht="18.75">
       <c r="B41" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D41" s="8">
         <f>(IF(D42="Know Well", 1, IF(D42="Know a Little", 0.5, 0))+IF(D43="Know Well", 1, IF(D43="Know a Little", 0.5, 0))+IF(D44="Know Well", 1, IF(D44="Know a Little", 0.5, 0))+IF(D45="Know Well", 1, IF(D45="Know a Little", 0.5, 0))+IF(D46="Know Well", 1, IF(D46="Know a Little", 0.5, 0)))/5</f>
@@ -3253,47 +3270,47 @@
     </row>
     <row r="42" spans="2:4" ht="15.75">
       <c r="C42" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D42" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="15.75">
       <c r="C43" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D43" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="15.75">
       <c r="C44" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D44" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="2:4" ht="15.75">
       <c r="C45" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D45" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="2:4" ht="15.75">
       <c r="C46" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D46" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="47" spans="2:4" s="7" customFormat="1" ht="18.75">
       <c r="B47" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D47" s="8">
         <f>(IF(D48="Know Well", 1, IF(D48="Know a Little", 0.5, 0))+IF(D49="Know Well", 1, IF(D49="Know a Little", 0.5, 0))+IF(D50="Know Well", 1, IF(D50="Know a Little", 0.5, 0))+IF(D51="Know Well", 1, IF(D51="Know a Little", 0.5, 0)))/4</f>
@@ -3302,39 +3319,39 @@
     </row>
     <row r="48" spans="2:4" ht="15.75">
       <c r="C48" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D48" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15.75">
       <c r="C49" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D49" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15.75">
       <c r="C50" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D50" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15.75">
       <c r="C51" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D51" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="52" spans="1:4" s="7" customFormat="1" ht="18.75">
       <c r="B52" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D52" s="8">
         <f>(IF(D53="Know Well", 1, IF(D53="Know a Little", 0.5, 0))+IF(D54="Know Well", 1, IF(D54="Know a Little", 0.5, 0))+IF(D55="Know Well", 1, IF(D55="Know a Little", 0.5, 0))+IF(D56="Know Well", 1, IF(D56="Know a Little", 0.5, 0))+IF(D57="Know Well", 1, IF(D57="Know a Little", 0.5, 0)))/5</f>
@@ -3343,42 +3360,42 @@
     </row>
     <row r="53" spans="1:4" ht="15.75">
       <c r="C53" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15.75">
       <c r="C54" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D54" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15.75">
       <c r="C55" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D55" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15.75">
       <c r="C56" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D56" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15.75">
       <c r="C57" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D57" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="58" spans="1:4" s="6" customFormat="1" ht="21">
@@ -3392,7 +3409,7 @@
     </row>
     <row r="59" spans="1:4" s="7" customFormat="1" ht="18.75">
       <c r="B59" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D59" s="8">
         <f>(IF(D60="Know Well", 1, IF(D60="Know a Little", 0.5, 0))+IF(D61="Know Well", 1, IF(D61="Know a Little", 0.5, 0))+IF(D62="Know Well", 1, IF(D62="Know a Little", 0.5, 0)))/3</f>
@@ -3401,31 +3418,31 @@
     </row>
     <row r="60" spans="1:4" ht="15.75">
       <c r="C60" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D60" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15.75">
       <c r="C61" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D61" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15.75">
       <c r="C62" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D62" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="63" spans="1:4" s="7" customFormat="1" ht="18.75">
       <c r="B63" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D63" s="8">
         <f>(IF(D64="Know Well", 1, IF(D64="Know a Little", 0.5, 0))+IF(D65="Know Well", 1, IF(D65="Know a Little", 0.5, 0))+IF(D66="Know Well", 1, IF(D66="Know a Little", 0.5, 0))+IF(D67="Know Well", 1, IF(D67="Know a Little", 0.5, 0))+IF(D68="Know Well", 1, IF(D68="Know a Little", 0.5, 0))+IF(D69="Know Well", 1, IF(D69="Know a Little", 0.5, 0)))/6</f>
@@ -3434,55 +3451,55 @@
     </row>
     <row r="64" spans="1:4" ht="15.75">
       <c r="C64" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D64" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="65" spans="2:4" ht="15.75">
       <c r="C65" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D65" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="66" spans="2:4" ht="15.75">
       <c r="C66" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D66" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="67" spans="2:4" ht="15.75">
       <c r="C67" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D67" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="68" spans="2:4" ht="15.75">
       <c r="C68" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D68" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="69" spans="2:4" ht="15.75">
       <c r="C69" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D69" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="70" spans="2:4" s="7" customFormat="1" ht="18.75">
       <c r="B70" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D70" s="8">
         <f>(IF(D71="Know Well", 1, IF(D71="Know a Little", 0.5, 0))+IF(D72="Know Well", 1, IF(D72="Know a Little", 0.5, 0))+IF(D73="Know Well", 1, IF(D73="Know a Little", 0.5, 0))+IF(D74="Know Well", 1, IF(D74="Know a Little", 0.5, 0))+IF(D75="Know Well", 1, IF(D75="Know a Little", 0.5, 0))+IF(D76="Know Well", 1, IF(D76="Know a Little", 0.5, 0))+IF(D77="Know Well", 1, IF(D77="Know a Little", 0.5, 0)))/7</f>
@@ -3491,63 +3508,63 @@
     </row>
     <row r="71" spans="2:4" ht="15.75">
       <c r="C71" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D71" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="72" spans="2:4" ht="15.75">
       <c r="C72" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D72" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="73" spans="2:4" ht="15.75">
       <c r="C73" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D73" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="74" spans="2:4" ht="15.75">
       <c r="C74" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D74" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="75" spans="2:4" ht="15.75">
       <c r="C75" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D75" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="76" spans="2:4" ht="15.75">
       <c r="C76" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D76" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="77" spans="2:4" ht="15.75">
       <c r="C77" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D77" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="78" spans="2:4" s="7" customFormat="1" ht="18.75">
       <c r="B78" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D78" s="8">
         <f>(IF(D79="Know Well", 1, IF(D79="Know a Little", 0.5, 0))+IF(D80="Know Well", 1, IF(D80="Know a Little", 0.5, 0))+IF(D81="Know Well", 1, IF(D81="Know a Little", 0.5, 0))+IF(D82="Know Well", 1, IF(D82="Know a Little", 0.5, 0))+IF(D83="Know Well", 1, IF(D83="Know a Little", 0.5, 0)))/5</f>
@@ -3556,47 +3573,47 @@
     </row>
     <row r="79" spans="2:4" ht="15.75">
       <c r="C79" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D79" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="80" spans="2:4" ht="15.75">
       <c r="C80" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D80" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15.75">
       <c r="C81" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D81" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="15.75">
       <c r="C82" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D82" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="15.75">
       <c r="C83" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D83" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="84" spans="1:4" s="6" customFormat="1" ht="21">
       <c r="A84" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D84" s="11">
         <f>SUM(D85:D106)/7</f>
@@ -3605,7 +3622,7 @@
     </row>
     <row r="85" spans="1:4" s="7" customFormat="1" ht="18.75">
       <c r="B85" s="7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D85" s="8">
         <f>(IF(D86="Know Well", 1, IF(D86="Know a Little", 0.5, 0))+IF(D87="Know Well", 1, IF(D87="Know a Little", 0.5, 0))+IF(D88="Know Well", 1, IF(D88="Know a Little", 0.5, 0))+IF(D89="Know Well", 1, IF(D89="Know a Little", 0.5, 0)))/4</f>
@@ -3614,39 +3631,39 @@
     </row>
     <row r="86" spans="1:4" ht="15.75">
       <c r="C86" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D86" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="15.75">
       <c r="C87" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D87" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="15.75">
       <c r="C88" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D88" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="15.75">
       <c r="C89" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D89" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="90" spans="1:4" s="7" customFormat="1" ht="18.75">
       <c r="B90" s="7" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D90" s="8">
         <f>(IF(D91="Know Well", 1, IF(D91="Know a Little", 0.5, 0)))/1</f>
@@ -3655,15 +3672,15 @@
     </row>
     <row r="91" spans="1:4" ht="15.75">
       <c r="C91" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D91" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="92" spans="1:4" s="7" customFormat="1" ht="18.75">
       <c r="B92" s="7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D92" s="8">
         <f>(IF(D93="Know Well", 1, IF(D93="Know a Little", 0.5, 0))+IF(D94="Know Well", 1, IF(D94="Know a Little", 0.5, 0))+IF(D95="Know Well", 1, IF(D95="Know a Little", 0.5, 0)))/3</f>
@@ -3672,31 +3689,31 @@
     </row>
     <row r="93" spans="1:4" ht="15.75">
       <c r="C93" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D93" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="15.75">
       <c r="C94" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D94" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="15.75">
       <c r="C95" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D95" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="96" spans="1:4" s="7" customFormat="1" ht="18.75">
       <c r="B96" s="7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D96" s="8">
         <f>(IF(D97="Know Well", 1, IF(D97="Know a Little", 0.5, 0))+IF(D98="Know Well", 1, IF(D98="Know a Little", 0.5, 0))+IF(D99="Know Well", 1, IF(D99="Know a Little", 0.5, 0))+IF(D100="Know Well", 1, IF(D100="Know a Little", 0.5, 0)))/4</f>
@@ -3705,39 +3722,39 @@
     </row>
     <row r="97" spans="1:4" ht="15.75">
       <c r="C97" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D97" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="15.75">
       <c r="C98" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D98" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="15.75">
       <c r="C99" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D99" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="15.75">
       <c r="C100" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D100" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="101" spans="1:4" s="7" customFormat="1" ht="18.75">
       <c r="B101" s="7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D101" s="8">
         <f>(IF(D102="Know Well", 1, IF(D102="Know a Little", 0.5, 0)))/1</f>
@@ -3746,15 +3763,15 @@
     </row>
     <row r="102" spans="1:4" ht="15.75">
       <c r="C102" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D102" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="103" spans="1:4" s="7" customFormat="1" ht="18.75">
       <c r="B103" s="7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D103" s="8">
         <f>(IF(D104="Know Well", 1, IF(D104="Know a Little", 0.5, 0)))/1</f>
@@ -3763,15 +3780,15 @@
     </row>
     <row r="104" spans="1:4" ht="15.75">
       <c r="C104" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D104" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="105" spans="1:4" s="7" customFormat="1" ht="18.75">
       <c r="B105" s="7" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D105" s="8">
         <f>(IF(D106="Know Well", 1, IF(D106="Know a Little", 0.5, 0)))/1</f>
@@ -3780,10 +3797,10 @@
     </row>
     <row r="106" spans="1:4" ht="15.75">
       <c r="C106" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D106" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="107" spans="1:4" s="6" customFormat="1" ht="21">
@@ -3797,7 +3814,7 @@
     </row>
     <row r="108" spans="1:4" s="7" customFormat="1" ht="18.75">
       <c r="B108" s="7" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D108" s="8">
         <f>(IF(D109="Know Well", 1, IF(D109="Know a Little", 0.5, 0))+IF(D110="Know Well", 1, IF(D110="Know a Little", 0.5, 0))+IF(D111="Know Well", 1, IF(D111="Know a Little", 0.5, 0))+IF(D112="Know Well", 1, IF(D112="Know a Little", 0.5, 0)))/4</f>
@@ -3806,39 +3823,39 @@
     </row>
     <row r="109" spans="1:4" ht="15.75">
       <c r="C109" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D109" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="15.75">
       <c r="C110" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D110" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="15.75">
       <c r="C111" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D111" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="15.75">
       <c r="C112" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D112" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="113" spans="2:4" s="7" customFormat="1" ht="18.75">
       <c r="B113" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D113" s="8">
         <f>(IF(D114="Know Well", 1, IF(D114="Know a Little", 0.5, 0))+IF(D115="Know Well", 1, IF(D115="Know a Little", 0.5, 0))+IF(D116="Know Well", 1, IF(D116="Know a Little", 0.5, 0))+IF(D117="Know Well", 1, IF(D117="Know a Little", 0.5, 0))+IF(D118="Know Well", 1, IF(D118="Know a Little", 0.5, 0)))/5</f>
@@ -3847,47 +3864,47 @@
     </row>
     <row r="114" spans="2:4" ht="15.75">
       <c r="C114" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D114" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="115" spans="2:4" ht="15.75">
       <c r="C115" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D115" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="116" spans="2:4" ht="15.75">
       <c r="C116" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D116" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="117" spans="2:4" ht="15.75">
       <c r="C117" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D117" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="118" spans="2:4" ht="15.75">
       <c r="C118" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D118" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="119" spans="2:4" s="7" customFormat="1" ht="18.75">
       <c r="B119" s="7" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D119" s="8">
         <f>(IF(D120="Know Well", 1, IF(D120="Know a Little", 0.5, 0))+IF(D121="Know Well", 1, IF(D121="Know a Little", 0.5, 0))+IF(D122="Know Well", 1, IF(D122="Know a Little", 0.5, 0))+IF(D123="Know Well", 1, IF(D123="Know a Little", 0.5, 0)))/4</f>
@@ -3896,39 +3913,39 @@
     </row>
     <row r="120" spans="2:4" ht="15.75">
       <c r="C120" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D120" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="121" spans="2:4" ht="15.75">
       <c r="C121" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D121" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="122" spans="2:4" ht="15.75">
       <c r="C122" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D122" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="123" spans="2:4" ht="15.75">
       <c r="C123" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D123" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="124" spans="2:4" s="7" customFormat="1" ht="18.75">
       <c r="B124" s="7" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D124" s="8">
         <f>(IF(D125="Know Well", 1, IF(D125="Know a Little", 0.5, 0)))/1</f>
@@ -3937,10 +3954,10 @@
     </row>
     <row r="125" spans="2:4" ht="15.75">
       <c r="C125" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D125" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -4784,22 +4801,22 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75">
       <c r="A1" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75">
       <c r="A2" s="4" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75">
       <c r="A3" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75">
       <c r="A4" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>